<commit_message>
add sprint goals and sprint backlog
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester 4\Pengembangan Perangkat Lunak Tangkas\Tugas UTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1305025A-F2EE-47A9-972E-D8422853A076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45378DF1-ACA5-4F8E-9701-ED89531F9D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
   <si>
     <t>Product Backlog &amp; User Story</t>
   </si>
@@ -63,19 +63,10 @@
     <t>Sprint Goals :</t>
   </si>
   <si>
-    <t>Seller can view product</t>
-  </si>
-  <si>
-    <t>….</t>
-  </si>
-  <si>
     <t>Sprint Backlog :</t>
   </si>
   <si>
     <t>Backlog Items</t>
-  </si>
-  <si>
-    <t>As a seller I want to view product …</t>
   </si>
   <si>
     <t>Sprint Review</t>
@@ -181,9 +172,6 @@
 DULU</t>
   </si>
   <si>
-    <t>TAMBAHKAN SPRINT 2, SPRINT 3 DST</t>
-  </si>
-  <si>
     <t>View recommended places</t>
   </si>
   <si>
@@ -278,6 +266,33 @@
   </si>
   <si>
     <t>LOW</t>
+  </si>
+  <si>
+    <t>Customer can save time</t>
+  </si>
+  <si>
+    <t>As a customer I want to enter the application without keep entering my personal information like bank account, etc</t>
+  </si>
+  <si>
+    <t>As a customer I want to view the most recommended places to holiday</t>
+  </si>
+  <si>
+    <t>Customers can choose the hotel they want</t>
+  </si>
+  <si>
+    <t>Customers feel comfortable while using the application</t>
+  </si>
+  <si>
+    <t>Customer can view the profile</t>
+  </si>
+  <si>
+    <t>Customer can easily see recommended places</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>As a customer, I want to see my profile information (name, profile picture, phone number, address, gender, email) on the profile screen.</t>
   </si>
 </sst>
 </file>
@@ -328,12 +343,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -402,20 +417,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -435,9 +441,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -452,41 +455,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -786,15 +798,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -821,21 +833,21 @@
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="2">
@@ -844,22 +856,22 @@
     </row>
     <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>54</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="G4" s="2">
         <v>3</v>
@@ -867,21 +879,21 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="2">
@@ -890,22 +902,22 @@
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="G6" s="2">
         <v>3</v>
@@ -913,22 +925,22 @@
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>58</v>
+        <v>67</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="G7" s="2">
         <v>3</v>
@@ -936,22 +948,22 @@
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>58</v>
+      <c r="F8" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="G8" s="2">
         <v>3</v>
@@ -959,323 +971,379 @@
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="G9" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="25" t="s">
-        <v>50</v>
-      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
+      <c r="A15" s="2">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="25">
+        <v>3</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="25"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
+      <c r="C20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="34" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="7">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="25"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="21"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="22"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="25"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="7">
-        <v>123</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="22"/>
+    </row>
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="25"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="32" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="7">
-        <v>1</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="B41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="22"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="24"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="24"/>
-    </row>
-    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="24"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="17" t="s">
+      <c r="B46" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17" t="s">
+      <c r="C46" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
+      <c r="D46" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="B47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="24"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+      <c r="D47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="24"/>
+      <c r="F47" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="F43:F47"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="G32:I34"/>
-    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="G34:I36"/>
     <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="F41:F45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1283,6 +1351,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100822B1C04D306CF40BAA48079013594C7" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0167222fc85e0d2d1ffbb9b2283bd68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="645225b3-beca-40ff-ac5d-71436c48a762" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d953b2bed9096f51fd31035f6cb08af" ns2:_="">
     <xsd:import namespace="645225b3-beca-40ff-ac5d-71436c48a762"/>
@@ -1408,16 +1485,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B9583CF-4A59-4C30-8DF2-417A621B0F41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B474253-CB26-41CF-8BA5-753D96C60926}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1433,12 +1509,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B9583CF-4A59-4C30-8DF2-417A621B0F41}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>